<commit_message>
Expanded test suite to 60 cases including boundary, negative, security and session scenarios
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,22 +486,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Valid user registration</t>
+          <t>Valid registration</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Enter valid name, email, phone, password and submit</t>
+          <t>Enter valid details and submit</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Name: John Doe, Email: john@test.com, Password: Test@123</t>
+          <t>Valid user data</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>User account created successfully</t>
+          <t>Account created successfully</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BR-03</t>
+          <t>BR-02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -533,27 +533,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Duplicate email registration</t>
+          <t>Invalid email format</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Register using existing email</t>
+          <t>Enter invalid email</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Existing email: john@test.com</t>
+          <t>abc@</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>System displays 'Email already exists' error</t>
+          <t>Validation error displayed</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BR-04</t>
+          <t>BR-03</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -580,27 +580,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Password less than 8 characters</t>
+          <t>Duplicate email</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Enter password with 6 characters</t>
+          <t>Register with existing email</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Pass: 123456</t>
+          <t>existing@test.com</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>System shows validation error</t>
+          <t>Email already exists error</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -617,37 +617,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BR-06</t>
+          <t>BR-04</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>Registration</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Valid login</t>
+          <t>Password less than 8 chars</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Enter correct email and password</t>
+          <t>Enter short password</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>john@test.com / Test@123</t>
+          <t>12345</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>User redirected to dashboard</t>
+          <t>Password validation error</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -664,37 +664,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BR-08</t>
+          <t>BR-04</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>Registration</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Account lock after 3 failed attempts</t>
+          <t>Password without number</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Enter wrong password 3 times</t>
+          <t>Enter password without digit</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>WrongPass123</t>
+          <t>Password</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Account locked for 15 minutes</t>
+          <t>Validation error</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -711,37 +711,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BR-10</t>
+          <t>BR-01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dashboard</t>
+          <t>Registration</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Verify account balance display</t>
+          <t>Blank name field</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Login and view dashboard</t>
+          <t>Leave name empty</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>User account with balance</t>
+          <t>Blank name</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Correct balance displayed</t>
+          <t>Mandatory field error</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -758,32 +758,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BR-11</t>
+          <t>BR-01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dashboard</t>
+          <t>Registration</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Verify last 5 transactions displayed</t>
+          <t>Blank email field</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Login and navigate to dashboard</t>
+          <t>Leave email empty</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Existing transaction data</t>
+          <t>Blank email</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Last 5 transactions visible</t>
+          <t>Mandatory field error</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -805,37 +805,37 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BR-14</t>
+          <t>BR-01</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Fund Transfer</t>
+          <t>Registration</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Transfer with sufficient balance</t>
+          <t>Blank password field</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Transfer 1000 to beneficiary with sufficient balance</t>
+          <t>Leave password empty</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Balance: 5000</t>
+          <t>Blank password</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Transfer successful and balance deducted</t>
+          <t>Mandatory field error</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -852,37 +852,37 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BR-14</t>
+          <t>BR-05</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Fund Transfer</t>
+          <t>Registration</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Transfer with insufficient balance</t>
+          <t>Confirmation email triggered</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Attempt transfer exceeding balance</t>
+          <t>Register successfully</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Balance: 500, Transfer: 2000</t>
+          <t>Valid data</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>System shows insufficient balance error</t>
+          <t>Confirmation email sent</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -899,37 +899,37 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BR-15</t>
+          <t>BR-02</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Fund Transfer</t>
+          <t>Registration</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Incorrect OTP during transfer</t>
+          <t>Special characters in email</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Enter wrong OTP during transaction</t>
+          <t>Enter special char email</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>OTP: 123456 (incorrect)</t>
+          <t>user@@bank</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Transfer not processed; error displayed</t>
+          <t>Validation error</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -946,37 +946,37 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BR-16</t>
+          <t>BR-06</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Fund Transfer</t>
+          <t>Login</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Balance deduction after successful OTP</t>
+          <t>Valid login</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Complete transfer with correct OTP</t>
+          <t>Enter correct credentials</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Valid OTP</t>
+          <t>Valid credentials</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Amount deducted and transaction recorded</t>
+          <t>Dashboard displayed</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -993,37 +993,37 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BR-18</t>
+          <t>BR-06</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Transaction History</t>
+          <t>Login</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>View transaction history</t>
+          <t>Invalid password</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Navigate to transaction history page</t>
+          <t>Enter wrong password</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Logged in user</t>
+          <t>Wrong pass</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>All transactions displayed correctly</t>
+          <t>Error displayed</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1040,37 +1040,37 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BR-19</t>
+          <t>BR-08</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Transaction History</t>
+          <t>Login</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Filter transactions by date</t>
+          <t>3 failed attempts lock</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Apply date filter</t>
+          <t>Enter wrong pass 3 times</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Date range: 01-01-2025 to 10-01-2025</t>
+          <t>Wrong pass</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Transactions filtered correctly</t>
+          <t>Account locked</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1087,37 +1087,37 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BR-20</t>
+          <t>BR-06</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Transaction History</t>
+          <t>Login</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Download transaction PDF</t>
+          <t>Blank password</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Click download PDF option</t>
+          <t>Leave password blank</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Logged in user</t>
+          <t>Blank</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>PDF downloaded successfully</t>
+          <t>Validation error</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1134,40 +1134,2155 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>BR-06</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Blank email</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Leave email blank</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Blank</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Validation error</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>TC_016</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BR-09</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Redirect after login</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Login successfully</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Valid login</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Redirect to dashboard</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TC_017</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>BR-08</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Login after lock period</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Wait 15 mins then login</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Valid credentials</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Login successful</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>TC_018</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BR-06</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>SQL injection attempt</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Enter SQL script in email</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>' OR 1=1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Login prevented</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TC_019</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>BR-06</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Case sensitivity check</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Enter case variation password</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Test@123 vs test@123</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Login should fail</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>TC_020</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BR-06</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Session created after login</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Login and inspect session</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Valid login</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Session ID generated</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>TC_021</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BR-10</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Balance display</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Login and check balance</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>User with balance</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Correct balance shown</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>TC_022</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>BR-11</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Last 5 transactions</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Check recent transactions</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>5 transactions displayed</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>TC_023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>BR-12</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Balance auto refresh</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Complete transfer</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Valid transfer</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Updated balance visible</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>TC_024</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BR-10</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Zero balance account</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Login zero balance user</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Balance 0</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0 displayed correctly</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>TC_025</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>BR-11</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>More than 5 transactions</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>User with 10 txns</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Only last 5 visible</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>TC_026</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>BR-10</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Negative balance display prevention</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Force negative balance</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Invalid scenario</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Negative not displayed</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>TC_027</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BR-10</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Large balance formatting</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>User with large balance</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>1,000,000</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Correct formatting</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>TC_028</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>BR-12</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Refresh page consistency</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Refresh dashboard</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Logged in</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Data remains consistent</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>TC_029</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>BR-10</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Unauthorized access</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Access dashboard without login</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Direct URL</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Redirect to login</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>TC_030</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>BR-11</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Dashboard</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Transaction order</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Check sorting</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Transaction list</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Sorted by latest first</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>TC_031</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Valid transfer with sufficient balance</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>TC_032</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Transfer exceeding balance</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>TC_033</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Incorrect OTP</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>TC_034</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Correct OTP</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>TC_035</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Transfer to invalid beneficiary</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>TC_036</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Transfer with blank amount</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>TC_037</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Transfer negative amount</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>TC_038</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Transfer zero amount</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>TC_039</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Large transfer boundary value</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>TC_040</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Session timeout during transfer</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>TC_041</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Double click submit button</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>TC_042</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Transfer with expired OTP</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>TC_043</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Transfer with special characters in amount</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>TC_044</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Transfer to self account</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>TC_045</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>BR-14</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Fund Transfer</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Balance deduction accuracy</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Perform transfer scenario</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Test data varies</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>System validates correctly</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>TC_046</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>View transaction history</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>TC_047</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Filter by valid date range</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>TC_048</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Filter by future date</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>TC_049</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Filter with invalid range</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>TC_050</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Download PDF</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>TC_051</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Download with no transactions</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>TC_052</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Large transaction list load</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>TC_053</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Sort by amount</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>TC_054</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Sort by date</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>TC_055</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>BR-18</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Transaction History</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Pagination validation</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Perform scenario</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Transaction data</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Correct output displayed</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>TC_056</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>BR-22</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>Logout</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Logout functionality</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Click logout button</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Logout normally</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Perform logout scenario</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
         <is>
           <t>Logged in session</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>User redirected to login page and session invalidated</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>User logged out securely</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>TC_057</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>BR-22</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Logout</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Access dashboard after logout</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Perform logout scenario</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Logged in session</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>User logged out securely</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TC_058</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>BR-22</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Logout</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Session invalid after logout</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Perform logout scenario</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Logged in session</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>User logged out securely</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>TC_059</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>BR-22</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Logout</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Multiple tab logout</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Perform logout scenario</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Logged in session</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>User logged out securely</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Not Executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>TC_060</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>BR-22</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Logout</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Session auto timeout after inactivity</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Perform logout scenario</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Logged in session</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>User logged out securely</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
         <is>
           <t>Not Executed</t>
         </is>

</xml_diff>